<commit_message>
added resume, pause, stop commands for music
</commit_message>
<xml_diff>
--- a/SFML_tester/Script Format Reference.xlsx
+++ b/SFML_tester/Script Format Reference.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\Debug\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D88DC04-1E4A-426B-836A-735FC41D07D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A4526E-70CE-4186-AA25-42FA5BE1FA39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>Line</t>
   </si>
@@ -94,30 +94,9 @@
     <t>Pause</t>
   </si>
   <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Dialogue</t>
-  </si>
-  <si>
     <t>Zoom</t>
   </si>
   <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
     <t>Wait/None</t>
   </si>
   <si>
@@ -127,9 +106,6 @@
     <t>Clockwise/Anticlockwise</t>
   </si>
   <si>
-    <t>Degree</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -142,18 +118,6 @@
     <t>choice2</t>
   </si>
   <si>
-    <t>Volume (optional)</t>
-  </si>
-  <si>
-    <t>Dialogue2(optional)</t>
-  </si>
-  <si>
-    <t>Dialogue3(optional)</t>
-  </si>
-  <si>
-    <t>Expression (Character) / Time-of-the-day (Background)</t>
-  </si>
-  <si>
     <t>Arg5</t>
   </si>
   <si>
@@ -205,9 +169,6 @@
     <t>Append</t>
   </si>
   <si>
-    <t>expression.mp3</t>
-  </si>
-  <si>
     <t>flag1</t>
   </si>
   <si>
@@ -260,6 +221,66 @@
   </si>
   <si>
     <t>StopLoop</t>
+  </si>
+  <si>
+    <t>BGM/SFX/Voice/All</t>
+  </si>
+  <si>
+    <t>[xPos=0]</t>
+  </si>
+  <si>
+    <t>[yPos=0]</t>
+  </si>
+  <si>
+    <t>[Time=0]</t>
+  </si>
+  <si>
+    <t>[y2]</t>
+  </si>
+  <si>
+    <t>[x1=0]</t>
+  </si>
+  <si>
+    <t>[y1=0]</t>
+  </si>
+  <si>
+    <t>[Volume=1]</t>
+  </si>
+  <si>
+    <t>[xScale=1]</t>
+  </si>
+  <si>
+    <t>[yScale=1]</t>
+  </si>
+  <si>
+    <t>[Degree]</t>
+  </si>
+  <si>
+    <t>[x2=0]</t>
+  </si>
+  <si>
+    <t>[Name]</t>
+  </si>
+  <si>
+    <t>[expression].mp3</t>
+  </si>
+  <si>
+    <t>[Expression].png</t>
+  </si>
+  <si>
+    <t>[Volume=0]</t>
+  </si>
+  <si>
+    <t>[Dialogue]</t>
+  </si>
+  <si>
+    <t>[Dialogue2(optional)]</t>
+  </si>
+  <si>
+    <t>[Dialogue3(optional)]</t>
+  </si>
+  <si>
+    <t>Resume</t>
   </si>
 </sst>
 </file>
@@ -690,22 +711,22 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -726,13 +747,13 @@
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -747,24 +768,24 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -773,19 +794,19 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -796,117 +817,117 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>10</v>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -920,58 +941,61 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
+      <c r="D13" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -982,19 +1006,19 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1005,73 +1029,73 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>18</v>
@@ -1079,10 +1103,10 @@
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>18</v>
@@ -1090,94 +1114,94 @@
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a bunch of new commands
</commit_message>
<xml_diff>
--- a/SFML_tester/Script Format Reference.xlsx
+++ b/SFML_tester/Script Format Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A4526E-70CE-4186-AA25-42FA5BE1FA39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE7FABB-053D-41BC-8A9A-BCB35F1DB136}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>Line</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Delay</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>Append</t>
   </si>
   <si>
@@ -281,6 +278,12 @@
   </si>
   <si>
     <t>Resume</t>
+  </si>
+  <si>
+    <t>[Time=0.5]</t>
+  </si>
+  <si>
+    <t>Wait/None/Relative/RelativeWait</t>
   </si>
 </sst>
 </file>
@@ -711,7 +714,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,19 +771,19 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -794,19 +797,19 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -817,28 +820,28 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -849,28 +852,28 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -881,22 +884,22 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -910,10 +913,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -927,7 +930,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -941,16 +944,16 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -958,13 +961,13 @@
         <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -972,30 +975,30 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>78</v>
+      <c r="D14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1009,16 +1012,16 @@
         <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1038,19 +1041,19 @@
         <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1058,16 +1061,16 @@
         <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1075,60 +1078,66 @@
         <v>35</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="D22" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="C23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>43</v>
+      <c r="D25" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>0</v>
@@ -1150,7 +1159,7 @@
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>24</v>
@@ -1159,32 +1168,32 @@
         <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>24</v>
@@ -1192,16 +1201,16 @@
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added skip mode (hold down CTRL keys to activate it)
</commit_message>
<xml_diff>
--- a/SFML_tester/Script Format Reference.xlsx
+++ b/SFML_tester/Script Format Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE7FABB-053D-41BC-8A9A-BCB35F1DB136}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B373F-5D13-4F85-8641-682D1A7A70A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AF088D-1F36-4E3F-BFB9-CD97E17BC052}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,35 +1024,35 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allowed multiple flags to be triggered for each choice
</commit_message>
<xml_diff>
--- a/SFML_tester/Script Format Reference.xlsx
+++ b/SFML_tester/Script Format Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63483DE-A005-4B5E-AC79-F23A5E91B869}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28478782-98B8-4710-A245-CD30296007F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>Line</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Append</t>
   </si>
   <si>
-    <t>flag1</t>
-  </si>
-  <si>
     <t>flag2</t>
   </si>
   <si>
@@ -305,6 +302,24 @@
   </si>
   <si>
     <t>flag expression (use &amp;, ^, !, () for logical expressions)</t>
+  </si>
+  <si>
+    <t>Blur</t>
+  </si>
+  <si>
+    <t>gradual? Relative?</t>
+  </si>
+  <si>
+    <t>start_blur</t>
+  </si>
+  <si>
+    <t>end_blur</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>flag1 (use comma (,) to separate mutliple flags)</t>
   </si>
 </sst>
 </file>
@@ -717,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AF088D-1F36-4E3F-BFB9-CD97E17BC052}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,19 +792,19 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -803,19 +818,19 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -826,28 +841,28 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -858,28 +873,28 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -890,22 +905,22 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -919,10 +934,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -936,98 +951,95 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>78</v>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1035,62 +1047,68 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1098,167 +1116,184 @@
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>63</v>
+      <c r="D22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="D27" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>58</v>
+      <c r="D33" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>